<commit_message>
Fix Excel, not ready yet
</commit_message>
<xml_diff>
--- a/registros.xlsx
+++ b/registros.xlsx
@@ -40,13 +40,13 @@
     <t>Sala de Computación</t>
   </si>
   <si>
-    <t>14/6/2025</t>
-  </si>
-  <si>
-    <t>José Pablo Yudico Martínez</t>
-  </si>
-  <si>
-    <t>21420237</t>
+    <t>15/6/2025</t>
+  </si>
+  <si>
+    <t>Yuriana Montserrat Ibarra Granados</t>
+  </si>
+  <si>
+    <t>21420209</t>
   </si>
   <si>
     <t>Ingeniería En Sistemas Computacionales</t>
@@ -509,17 +509,17 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>